<commit_message>
Criou o notebook digital_economic_outlook_2024_brasil_ocde.ipynb e alterou o arquivo governo_digital_brasil
</commit_message>
<xml_diff>
--- a/analise_dados/digital_economic_outlook_2024.xlsx
+++ b/analise_dados/digital_economic_outlook_2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lazar\Dissertacao-Mestrado-PoderJud-EGDI\analise_dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F6682F-6F1C-4B2E-858A-AAC9B1A87771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2888D40-27FC-45DD-9F38-DDBAB536998F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{4EE464EE-46C9-48B7-BF94-C9C1215358E0}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="40">
   <si>
     <t>Access</t>
   </si>
@@ -57,72 +57,6 @@
     <t>Market openness</t>
   </si>
   <si>
-    <t>BRA</t>
-  </si>
-  <si>
-    <t>CAN</t>
-  </si>
-  <si>
-    <t>CHE</t>
-  </si>
-  <si>
-    <t>COL</t>
-  </si>
-  <si>
-    <t>CZE</t>
-  </si>
-  <si>
-    <t>DEU</t>
-  </si>
-  <si>
-    <t>DNK</t>
-  </si>
-  <si>
-    <t>ESP</t>
-  </si>
-  <si>
-    <t>EST</t>
-  </si>
-  <si>
-    <t>FIN</t>
-  </si>
-  <si>
-    <t>GBR</t>
-  </si>
-  <si>
-    <t>HRV</t>
-  </si>
-  <si>
-    <t>HUN</t>
-  </si>
-  <si>
-    <t>IRL</t>
-  </si>
-  <si>
-    <t>JOR</t>
-  </si>
-  <si>
-    <t>JPN</t>
-  </si>
-  <si>
-    <t>LVA</t>
-  </si>
-  <si>
-    <t>MEX</t>
-  </si>
-  <si>
-    <t>NLD</t>
-  </si>
-  <si>
-    <t>NZL</t>
-  </si>
-  <si>
-    <t>SVK</t>
-  </si>
-  <si>
-    <t>SVN</t>
-  </si>
-  <si>
     <t>Czech Republic</t>
   </si>
   <si>
@@ -210,10 +144,16 @@
     <t>Permanent location of this file: https://stat.link/uyich5</t>
   </si>
   <si>
-    <t>Country Code</t>
-  </si>
-  <si>
-    <t>Country Name</t>
+    <t>OECD Membership</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Country</t>
   </si>
 </sst>
 </file>
@@ -631,23 +571,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31794806-DE5B-4514-94E6-EC9F3A5520FA}">
   <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.1796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1796875" style="1" customWidth="1"/>
     <col min="4" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>0</v>
@@ -677,10 +616,10 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="C2" s="8">
         <v>0.75</v>
@@ -715,10 +654,10 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="C3" s="8">
         <v>0.75</v>
@@ -752,10 +691,10 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="C4" s="8">
         <v>0</v>
@@ -789,10 +728,10 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="C5" s="8">
         <v>0.75</v>
@@ -826,10 +765,10 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="C6" s="8">
         <v>1</v>
@@ -863,10 +802,10 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="C7" s="10">
         <v>1</v>
@@ -900,10 +839,10 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="C8" s="10">
         <v>0</v>
@@ -937,10 +876,10 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>14</v>
+        <v>19</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="C9" s="10">
         <v>0.75</v>
@@ -974,10 +913,10 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>15</v>
+        <v>24</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="C10" s="10">
         <v>1</v>
@@ -1010,10 +949,10 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="C11" s="12">
         <v>0.5</v>
@@ -1046,10 +985,10 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="C12" s="12">
         <v>0.75</v>
@@ -1082,10 +1021,10 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="C13" s="12">
         <v>0.75</v>
@@ -1118,10 +1057,10 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="C14" s="12">
         <v>1</v>
@@ -1154,10 +1093,10 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="C15" s="12">
         <v>1</v>
@@ -1190,10 +1129,10 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="C16" s="12">
         <v>0.75</v>
@@ -1226,10 +1165,10 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="C17" s="12">
         <v>0.5</v>
@@ -1262,10 +1201,10 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="C18" s="12">
         <v>0.75</v>
@@ -1298,10 +1237,10 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="C19" s="12">
         <v>0.75</v>
@@ -1334,10 +1273,10 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="C20" s="12">
         <v>0.75</v>
@@ -1370,10 +1309,10 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>26</v>
+        <v>17</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="C21" s="12">
         <v>0.75</v>
@@ -1406,10 +1345,10 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>27</v>
+        <v>18</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="C22" s="12">
         <v>1</v>
@@ -1442,10 +1381,10 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="C23" s="12">
         <v>1</v>
@@ -1589,42 +1528,42 @@
   <sheetData>
     <row r="3" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B3" s="15" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B4" s="15" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B5" s="14" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B6" s="15" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B7" s="15" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B8" s="16" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B9" s="15" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B10" s="16" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>